<commit_message>
Updated API testing Code
Updated code for API testing by taking sample Billing Summary API
</commit_message>
<xml_diff>
--- a/Resources/TestData/B4C_TestData.xlsx
+++ b/Resources/TestData/B4C_TestData.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Selenium\XRay-JIRA-master\Resources\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work_Data\Selenium\DLGAutomationFramework\Resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5D18F14-6CD3-4423-8BF5-E79DC84A01A4}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510" xr2:uid="{0CAC76D4-88A8-4641-873F-588829D1B89F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510" tabRatio="716" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="GW_PC_AccountCreation" sheetId="1" r:id="rId1"/>
     <sheet name="GW_PC_SampleService" sheetId="2" r:id="rId2"/>
     <sheet name="GW_PC_GoogleSearch" sheetId="3" r:id="rId3"/>
+    <sheet name="GW_BC_BillingSummaryAPI" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="65">
   <si>
     <t>Feature</t>
   </si>
@@ -129,16 +129,117 @@
   </si>
   <si>
     <t>BR1 1PQ</t>
+  </si>
+  <si>
+    <t>PolicyNumber</t>
+  </si>
+  <si>
+    <t>TermNumber</t>
+  </si>
+  <si>
+    <t>EndPoint</t>
+  </si>
+  <si>
+    <t>http://10.109.11.67:8580/bc/ws/gw/webservice/policycenter/bc900/BillingSummaryAPI</t>
+  </si>
+  <si>
+    <t>2459765753</t>
+  </si>
+  <si>
+    <t>BillingStatus_BillingMethodCode</t>
+  </si>
+  <si>
+    <t>BillingStatus_Delinquent</t>
+  </si>
+  <si>
+    <t>BillingStatus_PastDue</t>
+  </si>
+  <si>
+    <t>BillingStatus_TotalBilled</t>
+  </si>
+  <si>
+    <t>BillingStatus_Unbilled</t>
+  </si>
+  <si>
+    <t>CurrentOutstanding</t>
+  </si>
+  <si>
+    <t>Invoices</t>
+  </si>
+  <si>
+    <t>Paid</t>
+  </si>
+  <si>
+    <t>PaymentPlanName</t>
+  </si>
+  <si>
+    <t>PolicyTermInfos_EffectiveDate</t>
+  </si>
+  <si>
+    <t>PolicyTermInfos_ExpirationDate</t>
+  </si>
+  <si>
+    <t>PolicyTermInfos_PolicyNumber</t>
+  </si>
+  <si>
+    <t>PolicyTermInfos_TermNumber</t>
+  </si>
+  <si>
+    <t>Retrieved</t>
+  </si>
+  <si>
+    <t>TotalCharges</t>
+  </si>
+  <si>
+    <t>WrittenOff</t>
+  </si>
+  <si>
+    <t>Archived</t>
+  </si>
+  <si>
+    <t>@DEMO-6</t>
+  </si>
+  <si>
+    <t>@DEMO-7</t>
+  </si>
+  <si>
+    <t>@DEMO-8</t>
+  </si>
+  <si>
+    <t>DirectBill</t>
+  </si>
+  <si>
+    <t>0 usd</t>
+  </si>
+  <si>
+    <t>0.00 usd</t>
+  </si>
+  <si>
+    <t>QA1PAYMENTPLAN10</t>
+  </si>
+  <si>
+    <t>2017-11-20T00:00:00+05:30</t>
+  </si>
+  <si>
+    <t>2018-11-20T00:00:00+05:30</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -161,14 +262,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -480,23 +584,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81D97047-87CC-45DD-9926-2B294CFD184E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7265625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -531,7 +635,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -557,7 +661,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -598,37 +702,37 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FE85618-B608-4915-9B9A-2B3657ECC27F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="S21" sqref="S21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB39FCA4-4627-4CBA-AD76-2B81C938D082}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:G1"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="13.7109375" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="13.7265625" customWidth="1"/>
+    <col min="7" max="7" width="10.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -651,7 +755,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -674,7 +778,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -697,7 +801,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -720,7 +824,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -746,4 +850,211 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Z2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="Q3" sqref="Q3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="5.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="75.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" customWidth="1"/>
+    <col min="11" max="11" width="28" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.26953125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.7265625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.90625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.54296875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.54296875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="26.453125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="27.81640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="27" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="26.6328125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J1" t="s">
+        <v>55</v>
+      </c>
+      <c r="K1" t="s">
+        <v>39</v>
+      </c>
+      <c r="L1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M1" t="s">
+        <v>41</v>
+      </c>
+      <c r="N1" t="s">
+        <v>42</v>
+      </c>
+      <c r="O1" t="s">
+        <v>43</v>
+      </c>
+      <c r="P1" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>45</v>
+      </c>
+      <c r="R1" t="s">
+        <v>46</v>
+      </c>
+      <c r="S1" t="s">
+        <v>47</v>
+      </c>
+      <c r="T1" t="s">
+        <v>48</v>
+      </c>
+      <c r="U1" t="s">
+        <v>49</v>
+      </c>
+      <c r="V1" t="s">
+        <v>50</v>
+      </c>
+      <c r="W1" t="s">
+        <v>51</v>
+      </c>
+      <c r="X1" t="s">
+        <v>52</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>53</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K2" t="s">
+        <v>59</v>
+      </c>
+      <c r="L2" t="b">
+        <v>0</v>
+      </c>
+      <c r="M2" t="s">
+        <v>60</v>
+      </c>
+      <c r="N2" t="s">
+        <v>61</v>
+      </c>
+      <c r="O2" t="s">
+        <v>61</v>
+      </c>
+      <c r="P2" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2" t="s">
+        <v>61</v>
+      </c>
+      <c r="S2" t="s">
+        <v>62</v>
+      </c>
+      <c r="T2" t="s">
+        <v>63</v>
+      </c>
+      <c r="U2" t="s">
+        <v>64</v>
+      </c>
+      <c r="V2" t="str">
+        <f>H2</f>
+        <v>2459765753</v>
+      </c>
+      <c r="W2">
+        <f>I2</f>
+        <v>1</v>
+      </c>
+      <c r="X2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Completed Account creation feature
Included assertions and saved the generated account id
</commit_message>
<xml_diff>
--- a/Resources/TestData/B4C_TestData.xlsx
+++ b/Resources/TestData/B4C_TestData.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work_Data\Selenium\DLGAutomationFramework\Resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510" tabRatio="716" activeTab="1"/>
+    <workbookView tabRatio="716" windowHeight="9510" windowWidth="24000" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="GW_PC_AccountCreation" sheetId="1" r:id="rId1"/>
-    <sheet name="GW_PC_GoogleSearch" sheetId="3" r:id="rId2"/>
-    <sheet name="GW_BC_BillingSummaryAPI" sheetId="4" r:id="rId3"/>
+    <sheet name="GW_PC_AccountCreation" r:id="rId1" sheetId="1"/>
+    <sheet name="GW_PC_GoogleSearch" r:id="rId2" sheetId="3"/>
+    <sheet name="GW_BC_BillingSummaryAPI" r:id="rId3" sheetId="4"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="75">
   <si>
     <t>Feature</t>
   </si>
@@ -109,124 +109,155 @@
     <t>Postcode</t>
   </si>
   <si>
-    <t>F_NAME</t>
-  </si>
-  <si>
-    <t>L_NAME</t>
-  </si>
-  <si>
-    <t>Automation</t>
+    <t>United Kingdom</t>
+  </si>
+  <si>
+    <t>Bromley</t>
+  </si>
+  <si>
+    <t>BR1 1PQ</t>
+  </si>
+  <si>
+    <t>PolicyNumber</t>
+  </si>
+  <si>
+    <t>TermNumber</t>
+  </si>
+  <si>
+    <t>EndPoint</t>
+  </si>
+  <si>
+    <t>http://10.109.11.67:8580/bc/ws/gw/webservice/policycenter/bc900/BillingSummaryAPI</t>
+  </si>
+  <si>
+    <t>2459765753</t>
+  </si>
+  <si>
+    <t>BillingStatus_BillingMethodCode</t>
+  </si>
+  <si>
+    <t>BillingStatus_Delinquent</t>
+  </si>
+  <si>
+    <t>BillingStatus_PastDue</t>
+  </si>
+  <si>
+    <t>BillingStatus_TotalBilled</t>
+  </si>
+  <si>
+    <t>BillingStatus_Unbilled</t>
+  </si>
+  <si>
+    <t>CurrentOutstanding</t>
+  </si>
+  <si>
+    <t>Invoices</t>
+  </si>
+  <si>
+    <t>Paid</t>
+  </si>
+  <si>
+    <t>PaymentPlanName</t>
+  </si>
+  <si>
+    <t>PolicyTermInfos_EffectiveDate</t>
+  </si>
+  <si>
+    <t>PolicyTermInfos_ExpirationDate</t>
+  </si>
+  <si>
+    <t>PolicyTermInfos_PolicyNumber</t>
+  </si>
+  <si>
+    <t>PolicyTermInfos_TermNumber</t>
+  </si>
+  <si>
+    <t>Retrieved</t>
+  </si>
+  <si>
+    <t>TotalCharges</t>
+  </si>
+  <si>
+    <t>WrittenOff</t>
+  </si>
+  <si>
+    <t>Archived</t>
+  </si>
+  <si>
+    <t>@DEMO-6</t>
+  </si>
+  <si>
+    <t>@DEMO-7</t>
+  </si>
+  <si>
+    <t>@DEMO-8</t>
+  </si>
+  <si>
+    <t>DirectBill</t>
+  </si>
+  <si>
+    <t>0 usd</t>
+  </si>
+  <si>
+    <t>0.00 usd</t>
+  </si>
+  <si>
+    <t>QA1PAYMENTPLAN10</t>
+  </si>
+  <si>
+    <t>2017-11-20T00:00:00+05:30</t>
+  </si>
+  <si>
+    <t>2018-11-20T00:00:00+05:30</t>
+  </si>
+  <si>
+    <t>Company</t>
+  </si>
+  <si>
+    <t>Address_1</t>
+  </si>
+  <si>
+    <t>London</t>
+  </si>
+  <si>
+    <t>Address_Type</t>
+  </si>
+  <si>
+    <t>Home</t>
+  </si>
+  <si>
+    <t>Organization</t>
+  </si>
+  <si>
+    <t>Producer_Code</t>
+  </si>
+  <si>
+    <t>Enigma Fire &amp; Casualty</t>
+  </si>
+  <si>
+    <t>dfgd</t>
+  </si>
+  <si>
+    <t>Account_ID</t>
+  </si>
+  <si>
+    <t>9706722468</t>
+  </si>
+  <si>
+    <t>Maven</t>
   </si>
   <si>
     <t>Demo</t>
   </si>
   <si>
-    <t>United Kingdom</t>
-  </si>
-  <si>
-    <t>Bromley</t>
-  </si>
-  <si>
-    <t>BR1 1PQ</t>
-  </si>
-  <si>
-    <t>PolicyNumber</t>
-  </si>
-  <si>
-    <t>TermNumber</t>
-  </si>
-  <si>
-    <t>EndPoint</t>
-  </si>
-  <si>
-    <t>http://10.109.11.67:8580/bc/ws/gw/webservice/policycenter/bc900/BillingSummaryAPI</t>
-  </si>
-  <si>
-    <t>2459765753</t>
-  </si>
-  <si>
-    <t>BillingStatus_BillingMethodCode</t>
-  </si>
-  <si>
-    <t>BillingStatus_Delinquent</t>
-  </si>
-  <si>
-    <t>BillingStatus_PastDue</t>
-  </si>
-  <si>
-    <t>BillingStatus_TotalBilled</t>
-  </si>
-  <si>
-    <t>BillingStatus_Unbilled</t>
-  </si>
-  <si>
-    <t>CurrentOutstanding</t>
-  </si>
-  <si>
-    <t>Invoices</t>
-  </si>
-  <si>
-    <t>Paid</t>
-  </si>
-  <si>
-    <t>PaymentPlanName</t>
-  </si>
-  <si>
-    <t>PolicyTermInfos_EffectiveDate</t>
-  </si>
-  <si>
-    <t>PolicyTermInfos_ExpirationDate</t>
-  </si>
-  <si>
-    <t>PolicyTermInfos_PolicyNumber</t>
-  </si>
-  <si>
-    <t>PolicyTermInfos_TermNumber</t>
-  </si>
-  <si>
-    <t>Retrieved</t>
-  </si>
-  <si>
-    <t>TotalCharges</t>
-  </si>
-  <si>
-    <t>WrittenOff</t>
-  </si>
-  <si>
-    <t>Archived</t>
-  </si>
-  <si>
-    <t>@DEMO-6</t>
-  </si>
-  <si>
-    <t>@DEMO-7</t>
-  </si>
-  <si>
-    <t>@DEMO-8</t>
-  </si>
-  <si>
-    <t>DirectBill</t>
-  </si>
-  <si>
-    <t>0 usd</t>
-  </si>
-  <si>
-    <t>0.00 usd</t>
-  </si>
-  <si>
-    <t>QA1PAYMENTPLAN10</t>
-  </si>
-  <si>
-    <t>2017-11-20T00:00:00+05:30</t>
-  </si>
-  <si>
-    <t>2018-11-20T00:00:00+05:30</t>
+    <t>0892109396</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -278,7 +309,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -301,30 +332,40 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+  <cellXfs count="12">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="1" fillId="2" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="1" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="1" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="4" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="1" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="1" fillId="4" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="1" fillId="4" fontId="1" numFmtId="0" xfId="1"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="2" fontId="2" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -341,10 +382,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -379,7 +420,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -431,7 +472,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -542,21 +583,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -573,7 +614,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -625,33 +666,39 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R3"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="13.7265625" collapsed="false"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="16.453125" collapsed="false"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="13.7265625" collapsed="false"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="12.0" collapsed="false"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="11.7265625" collapsed="false"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="9.08984375" collapsed="false"/>
+    <col min="9" max="9" customWidth="true" width="10.7265625" collapsed="false"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="14.1796875" collapsed="false"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="7.7265625" collapsed="false"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="9.54296875" collapsed="false"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="12.54296875" collapsed="false"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="19.90625" collapsed="false"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="13.81640625" collapsed="false"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="10.453125" collapsed="false"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>3</v>
       </c>
@@ -677,16 +724,34 @@
         <v>23</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>26</v>
       </c>
+      <c r="M1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="P1" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q1" s="11" t="s">
+        <v>70</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
         <v>4</v>
       </c>
@@ -705,17 +770,25 @@
       <c r="F2" s="8">
         <v>1</v>
       </c>
-      <c r="G2" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>28</v>
+      <c r="G2" s="5" t="str">
+        <f>G3</f>
+        <v>Maven</v>
+      </c>
+      <c r="H2" s="5" t="str">
+        <f>H3</f>
+        <v>Demo</v>
       </c>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
       <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
         <v>4</v>
       </c>
@@ -735,41 +808,59 @@
         <v>1</v>
       </c>
       <c r="G3" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L3" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="H3" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>33</v>
+      <c r="M3" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="O3" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="P3" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q3" s="5" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="13.7265625" customWidth="1"/>
-    <col min="7" max="7" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="13.7265625" collapsed="false"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="16.453125" collapsed="false"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="13.7265625" collapsed="false"/>
+    <col min="5" max="6" customWidth="true" width="13.7265625" collapsed="false"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="10.453125" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
@@ -888,13 +979,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AA2"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="J1" sqref="J1"/>
@@ -902,31 +993,31 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.08984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="75.1796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.36328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12" customWidth="1"/>
-    <col min="11" max="11" width="28" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.26953125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.7265625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.90625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.54296875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.54296875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.81640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="26.453125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="27.81640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="27" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="26.6328125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11.6328125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="6.7265625" collapsed="false"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="9.6328125" collapsed="false"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="15.26953125" collapsed="false"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.7265625" collapsed="false"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.0" collapsed="false"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="11.08984375" collapsed="false"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="75.1796875" collapsed="false"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="12.36328125" collapsed="false"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="12.0" collapsed="false"/>
+    <col min="10" max="10" customWidth="true" width="12.0" collapsed="false"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="28.0" collapsed="false"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="21.26953125" collapsed="false"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="18.81640625" collapsed="false"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="20.7265625" collapsed="false"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="18.90625" collapsed="false"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="17.54296875" collapsed="false"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="7.54296875" collapsed="false"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="7.81640625" collapsed="false"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="19.0" collapsed="false"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="26.453125" collapsed="false"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="27.81640625" collapsed="false"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="27.0" collapsed="false"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="26.6328125" collapsed="false"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="11.6328125" collapsed="false"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="9.81640625" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.35">
@@ -949,64 +1040,64 @@
         <v>17</v>
       </c>
       <c r="G1" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="L1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="K1" s="3" t="s">
+      <c r="M1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="O1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="W1" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="X1" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="Z1" s="3" t="s">
         <v>50</v>
-      </c>
-      <c r="W1" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="X1" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="Y1" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="Z1" s="3" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.35">
@@ -1014,13 +1105,13 @@
         <v>4</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E2" s="8">
         <v>1</v>
@@ -1029,10 +1120,10 @@
         <v>1</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="I2" s="5">
         <v>1</v>
@@ -1041,37 +1132,37 @@
         <v>0</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="L2" s="6" t="b">
         <v>0</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="O2" s="6" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="P2" s="6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="Q2" s="6">
         <v>0</v>
       </c>
       <c r="R2" s="6" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="S2" s="6" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="T2" s="6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="U2" s="6" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="V2" s="6" t="str">
         <f>H2</f>
@@ -1085,17 +1176,17 @@
         <v>0</v>
       </c>
       <c r="Y2" s="6" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="Z2" s="6" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1"/>
+    <hyperlink r:id="rId1" ref="G2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>